<commit_message>
Refactor code and added comments and also added test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testcase_Assignment2.xlsx
+++ b/src/test/resources/data/testcase_Assignment2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zop9604/Desktop/test evidence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zop9604/developer/git/Assignment/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF28387E-C73F-204C-8111-20042E52B70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A740EA-5ACE-9843-AD3E-61C55DBE2A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{D8AA799B-2A8B-C24F-B697-0664C7A22334}"/>
+    <workbookView xWindow="3300" yWindow="10000" windowWidth="27640" windowHeight="16940" xr2:uid="{D8AA799B-2A8B-C24F-B697-0664C7A22334}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
   <si>
     <t>Testing By: Gautam Gandhi</t>
   </si>
@@ -69,9 +69,6 @@
     <t xml:space="preserve">Sign in With InValid Credentials </t>
   </si>
   <si>
-    <t>Click on Forget Passoword</t>
-  </si>
-  <si>
     <t>Register New user when all the data fields have valid data</t>
   </si>
   <si>
@@ -96,38 +93,10 @@
     <t>Add one electronic to Wish list</t>
   </si>
   <si>
-    <t xml:space="preserve">Add none </t>
-  </si>
-  <si>
     <t>Adding none product to cart and validate cart</t>
   </si>
   <si>
-    <t>Adding none product to wishlist and validate cart</t>
-  </si>
-  <si>
-    <t>Add one computer to cart after adding all the valid fields</t>
-  </si>
-  <si>
-    <t>Add one computer to cart with processor drop down empty</t>
-  </si>
-  <si>
-    <t>Add one computer to cart with ram drop down empty</t>
-  </si>
-  <si>
-    <t>Add one computer to cart with hdd not selected</t>
-  </si>
-  <si>
-    <t>add 1million computer to cart with valid fields</t>
-  </si>
-  <si>
-    <t>add one computer and one electronic in compare list</t>
-  </si>
-  <si>
     <t>When Password is less than 6 character</t>
-  </si>
-  <si>
-    <t>End to end testing of one electronic and one computer with 
-payment from wishlist with different address</t>
   </si>
   <si>
     <t xml:space="preserve">End to end testing of one electronic and one computer with
@@ -156,33 +125,6 @@
   <si>
     <t>End to end testing of one electronic and one computer with
  payment after clicking I agree with zipcode contains character</t>
-  </si>
-  <si>
-    <t>"End to end testing of one electronic and one computer with
- payment after clicking I agree with empty mobile number</t>
-  </si>
-  <si>
-    <t>"End to end testing of one electronic and one computer with
- payment after clicking I agree with mobile number containing character</t>
-  </si>
-  <si>
-    <t>End to end testing of one electronic and one computer with
- payment after clicking I agree with zipcode contains 1 digit</t>
-  </si>
-  <si>
-    <t>End to end testing of one electronic and one computer with
- payment after clicking I agree with mobile number contains 
-1 digit</t>
-  </si>
-  <si>
-    <t>End to end testing of one electronic and one computer with
- payment after clicking I agree with all the valid details in 
-billing tab and next day air delivery</t>
-  </si>
-  <si>
-    <t>End to end testing of one electronic and one computer with
- payment after clicking I agree with all the valid details in 
-billing tab and second day air delivery</t>
   </si>
   <si>
     <t>End to end testing of one electronic and one computer with
@@ -190,9 +132,278 @@
 billing tab with ground deleivery option payment by check</t>
   </si>
   <si>
-    <t>End to end testing of one electronic and one computer with
- payment after clicking I agree with all the valid details in 
-billing tab with ground deleivery option payment by credit card</t>
+    <t>TC_1</t>
+  </si>
+  <si>
+    <t>1. navigate to url: https://demo.nopcommerce.com/
+2. click on login button.
+3. provide all the details.
+4. click on login button</t>
+  </si>
+  <si>
+    <t>email: abcde@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>Logout button appears on index page</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>TC_2</t>
+  </si>
+  <si>
+    <t>email: abcde10@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>Error message on login page "Login was unsuccessful. 
+Please correct the errors and try again.
+No customer account found"</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t>1. navigate to url: https://demo.nopcommerce.com/
+2. click on register button.
+3. provide all the details.
+4. click on register button</t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+LastName: pqrs
+email: abcde@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>Your registration completed message appears</t>
+  </si>
+  <si>
+    <t>TC_5</t>
+  </si>
+  <si>
+    <t>gender: female
+LastName: pqrs
+email: abcde@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>"First name is required." message appears</t>
+  </si>
+  <si>
+    <t>TC_6</t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+email: abcde@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>"Last name is required." message appears</t>
+  </si>
+  <si>
+    <t>TC_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register New user when inserted already existed Email Field </t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+LastName: pqrs
+email: abcde@gmail.com gautam@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>"The specified email already exists" 
+message appears</t>
+  </si>
+  <si>
+    <t>TC_8</t>
+  </si>
+  <si>
+    <t>Register New user when Email Field is Empty</t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+LastName: pqrs
+email: gautam@gmail.com
+password: 123456</t>
+  </si>
+  <si>
+    <t>TC_9</t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+LastName: pqrs
+email: abcde@gmail.com
+password:</t>
+  </si>
+  <si>
+    <t>"Password is required." message appears</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender: female
+FirstName: abcde
+LastName: pqrs
+email: abcde@gmail.com
+password: 123456
+confirm password: </t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+email: abcde@gmail.com
+password: 123456
+confirm password: 12345</t>
+  </si>
+  <si>
+    <t>"Password does not match" message appears</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>gender: female
+FirstName: abcde
+LastName: pqrs
+email: abcde@gmail.com
+password: 12345</t>
+  </si>
+  <si>
+    <t>"Password must be atleast 6 character." message appears</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>1. navigate to url: https://demo.nopcommerce.com/
+2. check the cart qty in index page</t>
+  </si>
+  <si>
+    <t>Qty = 0</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. navigate to url: https://demo.nopcommerce.com/
+2. click on electronic tab
+3. click on camera and photo
+4. click on DSLR camera
+5. click add to cart
+6. assert pop up message </t>
+  </si>
+  <si>
+    <t>The product has been added to your shopping cart message popup</t>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. navigate to url: https://demo.nopcommerce.com/
+2. click on electronic tab
+3. click on camera and photo
+4. click on DSLR camera
+5. click add to wishlist
+6. assert pop up message </t>
+  </si>
+  <si>
+    <t>The product has been added to your wishlist message popup</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>Add one computer to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. navigate to url: https://demo.nopcommerce.com/
+2. click on computer tab
+3. click on desktop
+4. click on Digital storm cpu
+5. click add to cart
+6. assert pop up message </t>
+  </si>
+  <si>
+    <t>TC_17</t>
+  </si>
+  <si>
+    <t>Add one computer to Wishlist</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>1. navigate to url: https://demo.nopcommerce.com/
+2. Add one electronic to cart.
+3. Add one computer to cart.
+4. navigate to cart</t>
+  </si>
+  <si>
+    <t>Two products appear in the cart</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>"Your order has been successfully processed!" after successfully 
+making payment</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>"Country cannot be empty" message</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>"State cannot be empty" message</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>"City cannot be empty" message</t>
+  </si>
+  <si>
+    <t>TC_23</t>
+  </si>
+  <si>
+    <t>"address1 cannot be empty" message</t>
+  </si>
+  <si>
+    <t>TC_24</t>
+  </si>
+  <si>
+    <t>"Zipcode cannot be empty" message</t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>character cannot be 
+inserted in zipcode</t>
   </si>
 </sst>
 </file>
@@ -558,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F87FDD-D147-F748-AACB-3557D3C6B509}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +780,7 @@
     <col min="3" max="3" width="52.1640625" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="55.5" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,193 +815,641 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
       <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+      <c r="D13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+      <c r="D14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C16" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="136" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
+      <c r="D26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
+      <c r="D28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
+      <c r="D30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+      <c r="D31" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C29" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C30" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C31" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C32" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C33" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C34" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C35" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C36" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C37" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C38" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C39" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C40" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C41" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C42" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="C43" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="C44" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="D33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>